<commit_message>
refactor: improve `_metadata.example.xlsx` wording + update accordingly build script/test
</commit_message>
<xml_diff>
--- a/knowledge/proprietary/_metadata.example.xlsx
+++ b/knowledge/proprietary/_metadata.example.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charnould/GitHub/pierre/knowledge/proprietary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5998610-6A18-EC43-8455-BF1FC6D6C8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0409846-E8FA-A84B-82D8-441C8B76975E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="1420" windowWidth="27500" windowHeight="17400" xr2:uid="{E5B0FB10-8797-D243-A0FA-6D923D5CC0EA}"/>
+    <workbookView xWindow="1200" yWindow="11080" windowWidth="27500" windowHeight="17400" xr2:uid="{E5B0FB10-8797-D243-A0FA-6D923D5CC0EA}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$2:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$3:$H$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>test-markdown-file.md</t>
   </si>
@@ -74,120 +74,219 @@
     <t>Ligne d'en-tête</t>
   </si>
   <si>
+    <t>Ci-après la procédure et la répartition des responsabilités entre la société de télésurveillance et l'agent/cadre d'astreinte chez Pierre Habitat :</t>
+  </si>
+  <si>
+    <t>Ci-après les noms des agents et cadre d'astreinte pour la semaine considérée chez Pierre Habitat :</t>
+  </si>
+  <si>
+    <t>Colonne de l'entité</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>building</t>
+  </si>
+  <si>
+    <t>Indiquer l'onglet concerné.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Doit correspondre </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>précisément</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> au chemin d'accès du fichier. Respecter les espaces et la casse.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Applicable uniquement aux fichiers .XLSX (Excel). </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sans effet pour les fichiers .DOCX (Word) et .MD (Markdown).</t>
+    </r>
+  </si>
+  <si>
+    <t>Segmentation</t>
+  </si>
+  <si>
+    <t>Parfois, il est davantage pertinent de considérer un fichier Excel non pas ligne par ligne, mais dans son ensemble.
+Mettre « false » pour que le tableau ne soit PAS segmenté, mais stocké en un seul « bloc ».</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+Optionnel, mais </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>important</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. 
+Afin d'aider PIERRE à comprendre le sujet couvert par l'onglet, indiquer avec les mots-clefs les plus pertinents à quoi correspond </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>une ligne du fichier Excel.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ci-après la description et les caractéristiques techniques d'une résidence de Pierre Habitat :</t>
+  </si>
+  <si>
+    <t>Ci-après les noms et coordonnées des collaborateurs en charge des résidences chez Pierre Habitat :</t>
+  </si>
+  <si>
+    <t>Type d'entité</t>
+  </si>
+  <si>
+    <t>Si l'onglet considéré contient un colonne relative à un programme immobilier (building) ou un processus (process), l'indiquer. 
+Sinon, laisser vide.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le contenu du fichier est-il </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>privé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (accessible avec un mot de passe) ou </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>public</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (accessible sans) ?</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">
-Qui a accès au contenu. Uniquement les collaborateurs (private) ou tout le monde (public).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Doit correspondre précisément au chemin d'accès du fichier. Respecter les espaces et la casse.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Applicable uniquement aux fichiers XLS. Indiquer l'onglet concerné.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Applicable uniquement aux fichiers XLS. Indiquer quelle est la ligne de la ligne d'en-têtes.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-Optionnelle, applicable principalement aux fichiers XLS mais </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>extrêmement important</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. Afin d'aider l'IA à comprendre le sujet couvert, indiquer le plus clairement possible à quoi correspond </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>une</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ligne du fichier Excel.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Ex : "Ci-après l'ensemble des élements et caractéristiques techniques d'une résidence de Pierre Habitat :"</t>
-    </r>
-  </si>
-  <si>
-    <t>Ci-après les caractéristiques techniques d'un programme immobilier de Pierre Habitat :</t>
-  </si>
-  <si>
-    <t>Ci-après les noms des collaborateurs en charge chez Pierre Habitat :</t>
-  </si>
-  <si>
-    <t>Ci-après la procédure et la répartition des responsabilités entre la société de télésurveillance et l'agent/cadre d'astreinte chez Pierre Habitat :</t>
-  </si>
-  <si>
-    <t>Ci-après les noms des agents et cadre d'astreinte pour la semaine considérée chez Pierre Habitat :</t>
-  </si>
-  <si>
-    <t>Colonne de l'entité</t>
-  </si>
-  <si>
-    <t>Type de l'entité</t>
-  </si>
-  <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>Découpage</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Applicable uniquement pour les fichiers XLS. Si le fichier est de petite taille ET qu'il fait davantage sens lorsqu'on le considère non pas ligne à ligne, mais globalement, mettre "false" ; il ne sera ainsi pas découper.</t>
+Indiquer à quelle ligne se trouve la ligne d'en-têtes (ex : pour ce fichier, la ligne d'entête est la 3).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Si vous avez renseigné </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>building</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ou </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> en colonne G, indiquer ici quelle est la colonne de l'entité (A = 1, B = 2, etc.)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,52 +295,146 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0070C0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF0070C0"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <u/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FF0070C0"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -256,22 +449,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,222 +815,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3359B2-613C-1246-BB58-A3F329ACACAC}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="101.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="55.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
+    <row r="1" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="202" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="76" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>24</v>
+      <c r="H2" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>2</v>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
+      <c r="D4" s="1">
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
+      <c r="H4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <v>3</v>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1">
-        <v>2</v>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
         <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H2" xr:uid="{0F3359B2-613C-1246-BB58-A3F329ACACAC}"/>
+  <autoFilter ref="A3:H3" xr:uid="{0F3359B2-613C-1246-BB58-A3F329ACACAC}"/>
   <dataConsolidate/>
-  <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C204" xr:uid="{49006576-7484-B84D-A51B-69FE1DA1041A}">
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:H1"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1001:E1679 D4:D1679" xr:uid="{49006576-7484-B84D-A51B-69FE1DA1041A}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{2D33CDDD-82FD-DF49-92A6-98CA2408197D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{2D33CDDD-82FD-DF49-92A6-98CA2408197D}">
       <formula1>"private,public"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G1679" xr:uid="{3055D0C6-D881-A443-AE4B-6D115C100895}">
+      <formula1>"building,process"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E1000" xr:uid="{1B35C915-B844-3A4E-8381-4D4F9C183493}">
+      <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>